<commit_message>
Se crea Enlace hacía curso
</commit_message>
<xml_diff>
--- a/Planificacion/Excel/CheckpointCursos_2023_V02.xlsx
+++ b/Planificacion/Excel/CheckpointCursos_2023_V02.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CCGQ095K\Documents\Udemy\udemy\Planificacion\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6D67F0-AAB6-4520-8082-A1F0BAB737C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6A984F-7AB8-4D94-B38F-3E74F3B40222}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cursos" sheetId="1" r:id="rId1"/>
@@ -2651,7 +2651,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17527,7 +17527,7 @@
         <v>0:00:00</v>
       </c>
       <c r="D2" s="127">
-        <f>B2-C2</f>
+        <f t="shared" ref="D2:D7" si="1">B2-C2</f>
         <v>1.4583333333333332E-2</v>
       </c>
       <c r="E2" s="126" t="s">
@@ -17545,7 +17545,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="123">
-        <f>B3-C3</f>
+        <f t="shared" si="1"/>
         <v>2.7777777777777779E-3</v>
       </c>
       <c r="E3" s="112" t="s">
@@ -17563,7 +17563,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="124">
-        <f>B4-C4</f>
+        <f t="shared" si="1"/>
         <v>2.0833333333333333E-3</v>
       </c>
       <c r="E4" s="112" t="s">
@@ -17581,7 +17581,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="124">
-        <f>B5-C5</f>
+        <f t="shared" si="1"/>
         <v>3.472222222222222E-3</v>
       </c>
       <c r="E5" s="112" t="s">
@@ -17599,7 +17599,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="124">
-        <f>B6-C6</f>
+        <f t="shared" si="1"/>
         <v>5.5555555555555558E-3</v>
       </c>
       <c r="E6" s="112" t="s">
@@ -17617,7 +17617,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="125">
-        <f>B7-C7</f>
+        <f t="shared" si="1"/>
         <v>6.9444444444444447E-4</v>
       </c>
       <c r="E7" s="112" t="s">
@@ -17635,7 +17635,7 @@
         <v>6.3194444444444442E-2</v>
       </c>
       <c r="D8" s="109">
-        <f t="shared" ref="D8:D20" si="1">B8-C8</f>
+        <f t="shared" ref="D8:D20" si="2">B8-C8</f>
         <v>0</v>
       </c>
       <c r="E8" s="126" t="s">
@@ -17653,7 +17653,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D9" s="111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E9" s="112" t="s">
@@ -17671,7 +17671,7 @@
         <v>4.8611111111111112E-3</v>
       </c>
       <c r="D10" s="111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.0555555555555555E-2</v>
       </c>
       <c r="E10" s="112" t="s">
@@ -17689,7 +17689,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.6527777777777779E-2</v>
       </c>
       <c r="E11" s="112" t="s">
@@ -17707,7 +17707,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.0416666666666667E-2</v>
       </c>
       <c r="E12" s="112" t="s">
@@ -17725,7 +17725,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.7916666666666663E-2</v>
       </c>
       <c r="E13" s="112" t="s">
@@ -17743,7 +17743,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.4305555555555555E-2</v>
       </c>
       <c r="E14" s="112" t="s">
@@ -17761,7 +17761,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.0555555555555555E-2</v>
       </c>
       <c r="E15" s="112" t="s">
@@ -17779,7 +17779,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9166666666666664E-2</v>
       </c>
       <c r="E16" s="112" t="s">
@@ -17797,7 +17797,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E17" s="112" t="s">
@@ -17815,7 +17815,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3194444444444444E-2</v>
       </c>
       <c r="E18" s="112" t="s">
@@ -17833,7 +17833,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.472222222222222E-3</v>
       </c>
       <c r="E19" s="112" t="s">
@@ -17851,7 +17851,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7361111111111112E-2</v>
       </c>
       <c r="E20" s="114" t="s">
@@ -25010,7 +25010,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -26359,8 +26361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F1104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
1. What you'll Get in This Course
</commit_message>
<xml_diff>
--- a/Planificacion/Excel/CheckpointCursos_2023_V02.xlsx
+++ b/Planificacion/Excel/CheckpointCursos_2023_V02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CCGQ095K\Documents\Udemy\udemy\Planificacion\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6A984F-7AB8-4D94-B38F-3E74F3B40222}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3121EB0B-5CEF-43E4-9F2C-53AAC4F71B4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2926,11 +2926,11 @@
       </c>
       <c r="D14" s="175" t="str">
         <f>TC2023WDB!C25</f>
-        <v>0:00:00</v>
+        <v>0:03:00</v>
       </c>
       <c r="E14" s="149" t="str">
         <f>TC2023WDB!D25</f>
-        <v>1:29:00</v>
+        <v>1:26:00</v>
       </c>
     </row>
     <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -25051,11 +25051,11 @@
       </c>
       <c r="C2" s="33" t="str">
         <f t="shared" si="0"/>
-        <v>0:00:00</v>
+        <v>0:03:00</v>
       </c>
       <c r="D2" s="34">
         <f t="shared" ref="D2:D20" si="1">B2-C2</f>
-        <v>2.6388888888888889E-2</v>
+        <v>2.4305555555555556E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -25066,11 +25066,11 @@
         <v>2.0833333333333333E-3</v>
       </c>
       <c r="C3" s="36">
-        <v>0</v>
+        <v>2.0833333333333333E-3</v>
       </c>
       <c r="D3" s="37">
         <f t="shared" si="1"/>
-        <v>2.0833333333333333E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -25366,11 +25366,11 @@
       </c>
       <c r="C25" s="42" t="str">
         <f t="shared" si="3"/>
-        <v>0:00:00</v>
+        <v>0:03:00</v>
       </c>
       <c r="D25" s="42" t="str">
         <f t="shared" si="3"/>
-        <v>1:29:00</v>
+        <v>1:26:00</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se sube nueva carpeta curso Lectura activa comprensiva
</commit_message>
<xml_diff>
--- a/Planificacion/Excel/CheckpointCursos_2023_V02.xlsx
+++ b/Planificacion/Excel/CheckpointCursos_2023_V02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CCGQ095K\Documents\Udemy\udemy\Planificacion\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0364E1EE-7325-470A-8AB7-55354B4FAA1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FBA568-00C9-4ACF-8A02-A37FCBB67EEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25010,9 +25010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>